<commit_message>
Version 5.1 edited as per user feedback to accept templates, populate graphics when pasted into excel
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Apps\Lieberman\StimuPop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F4E1C1-F993-4976-BC9F-B30FD6313122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0046934-7279-4783-AC75-108ACCC2943A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5604" yWindow="3804" windowWidth="19188" windowHeight="12240" xr2:uid="{BDDCAAAC-F496-4198-85C2-B86B95982EF7}"/>
   </bookViews>
@@ -462,7 +462,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>